<commit_message>
changes until 22-03, fix_Colombia with email sending
</commit_message>
<xml_diff>
--- a/outputs/colombia_fixed.xlsx
+++ b/outputs/colombia_fixed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="38">
   <si>
     <t>Departamento</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Antioquia</t>
   </si>
   <si>
+    <t>Archipiélago de San Andrés, Providencia y Santa Catalina</t>
+  </si>
+  <si>
     <t>Atlántico</t>
   </si>
   <si>
@@ -37,7 +40,13 @@
     <t>Caldas</t>
   </si>
   <si>
+    <t>Casanare</t>
+  </si>
+  <si>
     <t>Cauca</t>
+  </si>
+  <si>
+    <t>Cesar</t>
   </si>
   <si>
     <t>Cundinamarca</t>
@@ -116,6 +125,9 @@
   </si>
   <si>
     <t>21/03/2020</t>
+  </si>
+  <si>
+    <t>22/03/2020</t>
   </si>
 </sst>
 </file>
@@ -473,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C241"/>
+  <dimension ref="A1:C307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -506,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -517,7 +529,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -528,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -539,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -550,10 +562,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -561,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -572,7 +584,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -583,10 +595,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -594,7 +606,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -605,7 +617,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -616,7 +628,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -627,7 +639,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -638,7 +650,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -649,7 +661,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -657,10 +669,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -668,10 +680,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -679,10 +691,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -690,10 +702,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -701,10 +713,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -712,21 +724,21 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -734,10 +746,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -745,10 +757,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -756,10 +768,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -767,10 +779,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -778,21 +790,21 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -800,10 +812,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -811,10 +823,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -822,10 +834,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -833,10 +845,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -844,10 +856,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -855,10 +867,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -866,10 +878,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -877,21 +889,21 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -899,10 +911,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -910,10 +922,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -921,10 +933,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -932,10 +944,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -943,10 +955,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -954,10 +966,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -965,10 +977,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -976,32 +988,32 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1009,10 +1021,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1020,10 +1032,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1031,10 +1043,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1042,21 +1054,21 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1064,10 +1076,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1075,10 +1087,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1086,21 +1098,21 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1108,10 +1120,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1119,10 +1131,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1130,10 +1142,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1141,32 +1153,32 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1174,21 +1186,21 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1196,10 +1208,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1207,21 +1219,21 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1229,10 +1241,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1240,10 +1252,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1251,10 +1263,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1262,10 +1274,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1273,32 +1285,32 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1306,32 +1318,32 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C77">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -1339,21 +1351,21 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1361,10 +1373,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1372,21 +1384,21 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1394,10 +1406,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1405,10 +1417,10 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B85" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -1416,10 +1428,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -1427,10 +1439,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -1438,10 +1450,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -1449,10 +1461,10 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -1460,10 +1472,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -1471,10 +1483,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -1485,7 +1497,7 @@
         <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C92">
         <v>4</v>
@@ -1496,7 +1508,7 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -1507,10 +1519,10 @@
         <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1518,10 +1530,10 @@
         <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1529,7 +1541,7 @@
         <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -1540,10 +1552,10 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1551,10 +1563,10 @@
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1562,7 +1574,7 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -1573,10 +1585,10 @@
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1584,7 +1596,7 @@
         <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -1595,7 +1607,7 @@
         <v>13</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -1606,7 +1618,7 @@
         <v>14</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -1617,7 +1629,7 @@
         <v>15</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -1628,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -1639,29 +1651,29 @@
         <v>17</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C107">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -1669,10 +1681,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -1680,21 +1692,21 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -1702,32 +1714,32 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C112">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C113">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -1735,21 +1747,21 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -1757,10 +1769,10 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -1768,32 +1780,32 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -1801,32 +1813,32 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B122" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C122">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B123" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -1834,21 +1846,21 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B125" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -1856,10 +1868,10 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -1867,32 +1879,32 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B127" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C127">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B128" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C128">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -1900,32 +1912,32 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B130" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B132" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -1933,10 +1945,10 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B133" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -1944,10 +1956,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B134" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -1955,10 +1967,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -1966,32 +1978,32 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B136" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B137" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C137">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B138" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -1999,32 +2011,32 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B139" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B140" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B141" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -2032,32 +2044,32 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C142">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B143" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C143">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B144" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -2065,32 +2077,32 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B145" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B146" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B147" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -2098,32 +2110,32 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B148" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B149" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -2131,32 +2143,32 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B151" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C151">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B152" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C152">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B153" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -2164,32 +2176,32 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B154" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C154">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B155" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C155">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B156" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -2197,32 +2209,32 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B157" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C157">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B158" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C158">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B159" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -2230,32 +2242,32 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B160" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B161" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B162" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -2263,32 +2275,32 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B163" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B164" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -2296,65 +2308,65 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B166" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C166">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
+        <v>6</v>
+      </c>
+      <c r="B167" t="s">
+        <v>30</v>
+      </c>
+      <c r="C167">
         <v>3</v>
-      </c>
-      <c r="B167" t="s">
-        <v>29</v>
-      </c>
-      <c r="C167">
-        <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B168" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B169" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C169">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B170" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B171" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -2362,21 +2374,21 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B172" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C172">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B173" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C173">
         <v>7</v>
@@ -2384,10 +2396,10 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B174" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -2395,10 +2407,10 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B175" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -2406,21 +2418,21 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B176" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C176">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B177" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -2428,10 +2440,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B178" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -2439,21 +2451,21 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B179" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B180" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -2461,13 +2473,13 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B181" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C181">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2475,7 +2487,7 @@
         <v>3</v>
       </c>
       <c r="B182" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C182">
         <v>8</v>
@@ -2486,10 +2498,10 @@
         <v>4</v>
       </c>
       <c r="B183" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C183">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -2497,10 +2509,10 @@
         <v>5</v>
       </c>
       <c r="B184" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C184">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -2508,10 +2520,10 @@
         <v>6</v>
       </c>
       <c r="B185" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -2519,10 +2531,10 @@
         <v>7</v>
       </c>
       <c r="B186" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C186">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -2530,10 +2542,10 @@
         <v>8</v>
       </c>
       <c r="B187" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C187">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -2541,10 +2553,10 @@
         <v>9</v>
       </c>
       <c r="B188" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C188">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -2552,7 +2564,7 @@
         <v>10</v>
       </c>
       <c r="B189" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -2563,10 +2575,10 @@
         <v>11</v>
       </c>
       <c r="B190" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C190">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -2574,10 +2586,10 @@
         <v>12</v>
       </c>
       <c r="B191" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C191">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -2585,10 +2597,10 @@
         <v>13</v>
       </c>
       <c r="B192" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C192">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -2596,10 +2608,10 @@
         <v>14</v>
       </c>
       <c r="B193" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C193">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -2607,10 +2619,10 @@
         <v>15</v>
       </c>
       <c r="B194" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C194">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -2618,10 +2630,10 @@
         <v>16</v>
       </c>
       <c r="B195" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C195">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -2629,378 +2641,378 @@
         <v>17</v>
       </c>
       <c r="B196" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C196">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B197" t="s">
         <v>31</v>
       </c>
       <c r="C197">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B198" t="s">
         <v>31</v>
       </c>
       <c r="C198">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B199" t="s">
         <v>31</v>
       </c>
       <c r="C199">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B200" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C200">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B201" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C201">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B202" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C202">
-        <v>57</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B203" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C203">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B204" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B205" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C205">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B206" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C206">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B207" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C207">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B208" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C208">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B209" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C209">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B210" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C210">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B211" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C211">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B212" t="s">
         <v>32</v>
       </c>
       <c r="C212">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B213" t="s">
         <v>32</v>
       </c>
       <c r="C213">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B214" t="s">
         <v>32</v>
       </c>
       <c r="C214">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B215" t="s">
         <v>32</v>
       </c>
       <c r="C215">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B216" t="s">
         <v>32</v>
       </c>
       <c r="C216">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B217" t="s">
         <v>32</v>
       </c>
       <c r="C217">
-        <v>89</v>
+        <v>5</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B218" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C218">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B219" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C219">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B220" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C220">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B221" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C221">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B222" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C222">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B223" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C223">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B224" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C224">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B225" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C225">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B226" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C226">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B227" t="s">
         <v>33</v>
       </c>
       <c r="C227">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B228" t="s">
         <v>33</v>
       </c>
       <c r="C228">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B229" t="s">
         <v>33</v>
       </c>
       <c r="C229">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B230" t="s">
         <v>33</v>
@@ -3011,7 +3023,7 @@
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B231" t="s">
         <v>33</v>
@@ -3022,29 +3034,29 @@
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B232" t="s">
         <v>33</v>
       </c>
       <c r="C232">
-        <v>89</v>
+        <v>5</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B233" t="s">
         <v>33</v>
       </c>
       <c r="C233">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B234" t="s">
         <v>33</v>
@@ -3055,79 +3067,805 @@
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B235" t="s">
         <v>33</v>
       </c>
       <c r="C235">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B236" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C236">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B237" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C237">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B238" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C238">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B239" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C239">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B240" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C240">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
+        <v>8</v>
+      </c>
+      <c r="B241" t="s">
+        <v>34</v>
+      </c>
+      <c r="C241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" t="s">
+        <v>9</v>
+      </c>
+      <c r="B242" t="s">
+        <v>34</v>
+      </c>
+      <c r="C242">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" t="s">
+        <v>10</v>
+      </c>
+      <c r="B243" t="s">
+        <v>34</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" t="s">
+        <v>11</v>
+      </c>
+      <c r="B244" t="s">
+        <v>34</v>
+      </c>
+      <c r="C244">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" t="s">
+        <v>12</v>
+      </c>
+      <c r="B245" t="s">
+        <v>34</v>
+      </c>
+      <c r="C245">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" t="s">
+        <v>13</v>
+      </c>
+      <c r="B246" t="s">
+        <v>34</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" t="s">
+        <v>14</v>
+      </c>
+      <c r="B247" t="s">
+        <v>34</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" t="s">
+        <v>15</v>
+      </c>
+      <c r="B248" t="s">
+        <v>34</v>
+      </c>
+      <c r="C248">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" t="s">
+        <v>16</v>
+      </c>
+      <c r="B249" t="s">
+        <v>34</v>
+      </c>
+      <c r="C249">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" t="s">
         <v>17</v>
       </c>
-      <c r="B241" t="s">
-        <v>33</v>
-      </c>
-      <c r="C241">
+      <c r="B250" t="s">
+        <v>34</v>
+      </c>
+      <c r="C250">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" t="s">
+        <v>18</v>
+      </c>
+      <c r="B251" t="s">
+        <v>34</v>
+      </c>
+      <c r="C251">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
+        <v>19</v>
+      </c>
+      <c r="B252" t="s">
+        <v>34</v>
+      </c>
+      <c r="C252">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" t="s">
+        <v>20</v>
+      </c>
+      <c r="B253" t="s">
+        <v>34</v>
+      </c>
+      <c r="C253">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>35</v>
+      </c>
+      <c r="C254">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
+        <v>4</v>
+      </c>
+      <c r="B255" t="s">
+        <v>35</v>
+      </c>
+      <c r="C255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" t="s">
+        <v>5</v>
+      </c>
+      <c r="B256" t="s">
+        <v>35</v>
+      </c>
+      <c r="C256">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" t="s">
+        <v>6</v>
+      </c>
+      <c r="B257" t="s">
+        <v>35</v>
+      </c>
+      <c r="C257">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" t="s">
+        <v>7</v>
+      </c>
+      <c r="B258" t="s">
+        <v>35</v>
+      </c>
+      <c r="C258">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" t="s">
+        <v>8</v>
+      </c>
+      <c r="B259" t="s">
+        <v>35</v>
+      </c>
+      <c r="C259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" t="s">
+        <v>9</v>
+      </c>
+      <c r="B260" t="s">
+        <v>35</v>
+      </c>
+      <c r="C260">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" t="s">
+        <v>10</v>
+      </c>
+      <c r="B261" t="s">
+        <v>35</v>
+      </c>
+      <c r="C261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" t="s">
+        <v>11</v>
+      </c>
+      <c r="B262" t="s">
+        <v>35</v>
+      </c>
+      <c r="C262">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" t="s">
+        <v>12</v>
+      </c>
+      <c r="B263" t="s">
+        <v>35</v>
+      </c>
+      <c r="C263">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" t="s">
+        <v>13</v>
+      </c>
+      <c r="B264" t="s">
+        <v>35</v>
+      </c>
+      <c r="C264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" t="s">
+        <v>14</v>
+      </c>
+      <c r="B265" t="s">
+        <v>35</v>
+      </c>
+      <c r="C265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" t="s">
+        <v>15</v>
+      </c>
+      <c r="B266" t="s">
+        <v>35</v>
+      </c>
+      <c r="C266">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
+        <v>16</v>
+      </c>
+      <c r="B267" t="s">
+        <v>35</v>
+      </c>
+      <c r="C267">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>17</v>
+      </c>
+      <c r="B268" t="s">
+        <v>35</v>
+      </c>
+      <c r="C268">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" t="s">
+        <v>18</v>
+      </c>
+      <c r="B269" t="s">
+        <v>35</v>
+      </c>
+      <c r="C269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>19</v>
+      </c>
+      <c r="B270" t="s">
+        <v>35</v>
+      </c>
+      <c r="C270">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>20</v>
+      </c>
+      <c r="B271" t="s">
+        <v>35</v>
+      </c>
+      <c r="C271">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
+        <v>3</v>
+      </c>
+      <c r="B272" t="s">
+        <v>36</v>
+      </c>
+      <c r="C272">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>4</v>
+      </c>
+      <c r="B273" t="s">
+        <v>36</v>
+      </c>
+      <c r="C273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>5</v>
+      </c>
+      <c r="B274" t="s">
+        <v>36</v>
+      </c>
+      <c r="C274">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>6</v>
+      </c>
+      <c r="B275" t="s">
+        <v>36</v>
+      </c>
+      <c r="C275">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>7</v>
+      </c>
+      <c r="B276" t="s">
+        <v>36</v>
+      </c>
+      <c r="C276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
+        <v>8</v>
+      </c>
+      <c r="B277" t="s">
+        <v>36</v>
+      </c>
+      <c r="C277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
+        <v>9</v>
+      </c>
+      <c r="B278" t="s">
+        <v>36</v>
+      </c>
+      <c r="C278">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
+        <v>10</v>
+      </c>
+      <c r="B279" t="s">
+        <v>36</v>
+      </c>
+      <c r="C279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>11</v>
+      </c>
+      <c r="B280" t="s">
+        <v>36</v>
+      </c>
+      <c r="C280">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
+        <v>12</v>
+      </c>
+      <c r="B281" t="s">
+        <v>36</v>
+      </c>
+      <c r="C281">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
+        <v>13</v>
+      </c>
+      <c r="B282" t="s">
+        <v>36</v>
+      </c>
+      <c r="C282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" t="s">
+        <v>14</v>
+      </c>
+      <c r="B283" t="s">
+        <v>36</v>
+      </c>
+      <c r="C283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" t="s">
+        <v>15</v>
+      </c>
+      <c r="B284" t="s">
+        <v>36</v>
+      </c>
+      <c r="C284">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" t="s">
+        <v>16</v>
+      </c>
+      <c r="B285" t="s">
+        <v>36</v>
+      </c>
+      <c r="C285">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" t="s">
+        <v>17</v>
+      </c>
+      <c r="B286" t="s">
+        <v>36</v>
+      </c>
+      <c r="C286">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>18</v>
+      </c>
+      <c r="B287" t="s">
+        <v>36</v>
+      </c>
+      <c r="C287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>19</v>
+      </c>
+      <c r="B288" t="s">
+        <v>36</v>
+      </c>
+      <c r="C288">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" t="s">
+        <v>20</v>
+      </c>
+      <c r="B289" t="s">
+        <v>36</v>
+      </c>
+      <c r="C289">
         <v>26</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
+        <v>3</v>
+      </c>
+      <c r="B290" t="s">
+        <v>37</v>
+      </c>
+      <c r="C290">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" t="s">
+        <v>4</v>
+      </c>
+      <c r="B291" t="s">
+        <v>37</v>
+      </c>
+      <c r="C291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" t="s">
+        <v>5</v>
+      </c>
+      <c r="B292" t="s">
+        <v>37</v>
+      </c>
+      <c r="C292">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" t="s">
+        <v>6</v>
+      </c>
+      <c r="B293" t="s">
+        <v>37</v>
+      </c>
+      <c r="C293">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" t="s">
+        <v>7</v>
+      </c>
+      <c r="B294" t="s">
+        <v>37</v>
+      </c>
+      <c r="C294">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" t="s">
+        <v>8</v>
+      </c>
+      <c r="B295" t="s">
+        <v>37</v>
+      </c>
+      <c r="C295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" t="s">
+        <v>9</v>
+      </c>
+      <c r="B296" t="s">
+        <v>37</v>
+      </c>
+      <c r="C296">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" t="s">
+        <v>10</v>
+      </c>
+      <c r="B297" t="s">
+        <v>37</v>
+      </c>
+      <c r="C297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" t="s">
+        <v>11</v>
+      </c>
+      <c r="B298" t="s">
+        <v>37</v>
+      </c>
+      <c r="C298">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" t="s">
+        <v>12</v>
+      </c>
+      <c r="B299" t="s">
+        <v>37</v>
+      </c>
+      <c r="C299">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" t="s">
+        <v>13</v>
+      </c>
+      <c r="B300" t="s">
+        <v>37</v>
+      </c>
+      <c r="C300">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" t="s">
+        <v>14</v>
+      </c>
+      <c r="B301" t="s">
+        <v>37</v>
+      </c>
+      <c r="C301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" t="s">
+        <v>15</v>
+      </c>
+      <c r="B302" t="s">
+        <v>37</v>
+      </c>
+      <c r="C302">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" t="s">
+        <v>16</v>
+      </c>
+      <c r="B303" t="s">
+        <v>37</v>
+      </c>
+      <c r="C303">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" t="s">
+        <v>17</v>
+      </c>
+      <c r="B304" t="s">
+        <v>37</v>
+      </c>
+      <c r="C304">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" t="s">
+        <v>18</v>
+      </c>
+      <c r="B305" t="s">
+        <v>37</v>
+      </c>
+      <c r="C305">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" t="s">
+        <v>19</v>
+      </c>
+      <c r="B306" t="s">
+        <v>37</v>
+      </c>
+      <c r="C306">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" t="s">
+        <v>20</v>
+      </c>
+      <c r="B307" t="s">
+        <v>37</v>
+      </c>
+      <c r="C307">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>